<commit_message>
Convert: US9430_04_TransferQuote from ITG2 - ITG4
</commit_message>
<xml_diff>
--- a/data/US9430_04.xlsx
+++ b/data/US9430_04.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosaljah\OneDrive - Hewlett Packard Enterprise\TAO\ngq-demo-develop\ngq-demo-develop\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13848" windowHeight="6564"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13845" windowHeight="6570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,22 +19,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>strQuotenumber</t>
-  </si>
-  <si>
-    <t>NI00155727</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>TransferReason</t>
+  </si>
+  <si>
+    <t>TargetUser</t>
+  </si>
+  <si>
+    <t>UserGroup</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Encore CSR Group</t>
+  </si>
+  <si>
+    <t>ting-lan.luo@hpe.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF800000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -62,13 +84,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -339,7 +365,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -347,25 +373,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>